<commit_message>
createsp can add image by id
</commit_message>
<xml_diff>
--- a/sp_output3.xlsx
+++ b/sp_output3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
   <si>
     <t>0</t>
   </si>
@@ -385,13 +385,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,11 +401,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>103390</v>
       </c>
@@ -415,11 +412,8 @@
       <c r="C2">
         <v>113317</v>
       </c>
-      <c r="D2">
-        <v>104827</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1005525</v>
       </c>
@@ -429,11 +423,8 @@
       <c r="C3">
         <v>121782</v>
       </c>
-      <c r="D3">
-        <v>127918</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>102419</v>
       </c>
@@ -443,7 +434,19 @@
       <c r="C4">
         <v>102264</v>
       </c>
-      <c r="D4">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5">
+        <v>104827</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6">
+        <v>127918</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7">
         <v>125132</v>
       </c>
     </row>

</xml_diff>